<commit_message>
Making phone numbers clickable
</commit_message>
<xml_diff>
--- a/dataset/Daily sales/ds_excel/2023/Dailysales_07_2023.xlsx
+++ b/dataset/Daily sales/ds_excel/2023/Dailysales_07_2023.xlsx
@@ -639,16 +639,16 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>375</v>
+        <v>390</v>
       </c>
       <c r="C11" t="n">
-        <v>515</v>
+        <v>525</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
@@ -658,16 +658,16 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2787</v>
+        <v>2802</v>
       </c>
       <c r="C12" t="n">
-        <v>3924</v>
+        <v>3934</v>
       </c>
       <c r="D12" t="n">
         <v>15</v>
       </c>
       <c r="E12" t="n">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>